<commit_message>
feat: add tech-configuration tab and fix i18n issues
- Add new "Technical Configuration" tab to arena detail pages
  - Extract content from Tech Configuration.docx
  - Display with card-based layout matching implementation style
  - Support both English and Chinese versions

- Fix champion/擂主 badge display in arena pages
  - Fix conditional expression priority in client-page.tsx
  - Fix conditional expression priority in arena-client.tsx
  - Now properly displays trophy icon and gradient card for both languages

- Fix Chinese content showing English text in arena pages
  - Fix time display (1 week -> 一周, 1-2 days -> 1~2天)
  - Fix highlights display in arena detail pages
  - Update translateSpeedToTime to respect locale

- Add privacy policy and terms pages
- Add partner logos (logo7, logo8)
- Update email references to xuyuyao@tsinghua.edu.cn
- Sync content files for all pages

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Content/Arena/List of Arenas.xlsx
+++ b/Content/Arena/List of Arenas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20700" windowHeight="10275"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="78">
   <si>
     <t>擂台编号</t>
   </si>
@@ -64,7 +64,7 @@
     <t>成本</t>
   </si>
   <si>
-    <t>一周搭建企业级智能调研报告生成系统Demo</t>
+    <t>智能调研报告生成</t>
   </si>
   <si>
     <r>
@@ -222,7 +222,7 @@
     </r>
   </si>
   <si>
-    <t>较快</t>
+    <t>一周</t>
   </si>
   <si>
     <t>较高</t>
@@ -231,7 +231,7 @@
     <t>较优</t>
   </si>
   <si>
-    <t>两天搭建业务看板及网站Demo</t>
+    <t>业务看板搭建</t>
   </si>
   <si>
     <r>
@@ -369,13 +369,16 @@
     </r>
   </si>
   <si>
+    <t>1~2天</t>
+  </si>
+  <si>
     <t>很高</t>
   </si>
   <si>
     <t>较低</t>
   </si>
   <si>
-    <t>一周搭建文档审核与风控Demo</t>
+    <t>文档审核与风控</t>
   </si>
   <si>
     <r>
@@ -548,10 +551,7 @@
     </r>
   </si>
   <si>
-    <t>很快</t>
-  </si>
-  <si>
-    <t>两天半搭建企业级简要演示视频</t>
+    <t>企业演示视频</t>
   </si>
   <si>
     <r>
@@ -653,7 +653,7 @@
     <t>中等</t>
   </si>
   <si>
-    <t>一周搭建儿童教育趣味应用Demo</t>
+    <t>儿童教育趣味应用</t>
   </si>
   <si>
     <r>
@@ -728,7 +728,7 @@
     <t>服务</t>
   </si>
   <si>
-    <t>一周搭建长时间序列预测系统Demo（能源领域）</t>
+    <t>长时间序列预测系统</t>
   </si>
   <si>
     <r>
@@ -803,7 +803,7 @@
     </r>
   </si>
   <si>
-    <t>一周搭建智能文档翻译系统Demo</t>
+    <t>智能文档翻译系统</t>
   </si>
   <si>
     <r>
@@ -864,7 +864,7 @@
     </r>
   </si>
   <si>
-    <t>一天构建一个多合同交叉校验的智能合同法审系统Demo</t>
+    <t>智能合同法审系统</t>
   </si>
   <si>
     <r>
@@ -916,7 +916,7 @@
     <t>风控</t>
   </si>
   <si>
-    <t>一周搭建高精度通用目标检测系统Demo（能源&amp;农林领域）</t>
+    <t>通用目标检测系统</t>
   </si>
   <si>
     <r>
@@ -1107,7 +1107,24 @@
     </r>
   </si>
   <si>
-    <t>SQL语言智能生成(NL2SQL)的通用实践</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>语言智能生成</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1189,7 +1206,7 @@
     <t>信息技术</t>
   </si>
   <si>
-    <t>一周搭建对话式功能推荐助手Demo（AI领域）</t>
+    <t>功能推荐助手</t>
   </si>
   <si>
     <r>
@@ -1290,7 +1307,7 @@
     </r>
   </si>
   <si>
-    <t>一周构建智能信贷报告生成系统Demo</t>
+    <t>智能信贷报告生成系统</t>
   </si>
   <si>
     <r>
@@ -1333,7 +1350,7 @@
     </r>
   </si>
   <si>
-    <t>一周构建单条全国产业链图谱</t>
+    <t>单条产业链图谱</t>
   </si>
   <si>
     <t>一周低代码完成单条全国产业链图谱全流程构建</t>
@@ -1366,9 +1383,6 @@
       </rPr>
       <t>能源制造</t>
     </r>
-  </si>
-  <si>
-    <t>较慢</t>
   </si>
   <si>
     <r>
@@ -1401,7 +1415,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1597,6 +1611,12 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2438,8 +2458,8 @@
   <sheetPr/>
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2483,7 +2503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="14.25" spans="2:12">
+    <row r="4" spans="2:12">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -2554,13 +2574,13 @@
         <v>24</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>19</v>
@@ -2571,25 +2591,25 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>18</v>
@@ -2637,7 +2657,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>37</v>
@@ -2685,7 +2705,7 @@
         <v>42</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>37</v>
@@ -2781,7 +2801,7 @@
         <v>16</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>37</v>
@@ -2806,7 +2826,7 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" ht="14.25" spans="2:12">
+    <row r="17" spans="2:12">
       <c r="B17" s="3">
         <v>8</v>
       </c>
@@ -2829,7 +2849,7 @@
         <v>56</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>37</v>
@@ -2877,7 +2897,7 @@
         <v>61</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>37</v>
@@ -2912,7 +2932,7 @@
         <v>42</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>18</v>
@@ -2924,7 +2944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" ht="14.25" spans="2:12">
+    <row r="21" spans="2:12">
       <c r="B21" s="3">
         <v>11</v>
       </c>
@@ -2947,10 +2967,10 @@
         <v>70</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>18</v>
@@ -2995,7 +3015,7 @@
         <v>70</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>37</v>
@@ -3030,7 +3050,7 @@
         <v>70</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>37</v>
@@ -3047,7 +3067,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3151,19 +3171,19 @@
     <mergeCell ref="L21:L22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="一周搭建企业级智能调研报告生成系统Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/DbbUwFE8FiYjupki6uzcRqT0nEe?from=from_copylink"/>
-    <hyperlink ref="C6" r:id="rId2" display="两天搭建业务看板及网站Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/CtjuwGhsIiE977kD7TLc4u0KnRe?from=from_copylink"/>
-    <hyperlink ref="C7" r:id="rId3" display="一周搭建文档审核与风控Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/PQ6MwPExLi3v2Vkn3DAckYxGn8b?from=from_copylink"/>
-    <hyperlink ref="C9" r:id="rId4" display="两天半搭建企业级简要演示视频" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/Dkl8wQ6fBiE49Gk4XE2cTRc2nhD?from=from_copylink"/>
-    <hyperlink ref="C11" r:id="rId5" display="一周搭建儿童教育趣味应用Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/Csk3wFuMwiZk00kt8WJco88Wn5g?from=from_copylink"/>
-    <hyperlink ref="C13" r:id="rId6" display="一周搭建长时间序列预测系统Demo（能源领域）" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/G6S3wY1eriHk3UkfCDlc6PEznpd?from=from_copylink"/>
-    <hyperlink ref="C15" r:id="rId7" display="一周搭建智能文档翻译系统Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/QHljw6HhbiceMPkBC49cmvzNnXf?from=from_copylink"/>
-    <hyperlink ref="C17" r:id="rId8" display="一天构建一个多合同交叉校验的智能合同法审系统Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/NfpfwmK16iXEDtkznIscn549nEb?from=from_copylink"/>
-    <hyperlink ref="C19" r:id="rId9" display="一周搭建高精度通用目标检测系统Demo（能源&amp;农林领域）" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/OfMfwwUxMic5Qkkul8GcaA5En4d?from=from_copylink"/>
-    <hyperlink ref="C20" r:id="rId10" display="SQL语言智能生成(NL2SQL)的通用实践" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/GGMKw7bP7iXmNpk88OxcsqCznmg?from=from_copylink"/>
-    <hyperlink ref="C21" r:id="rId11" display="一周搭建对话式功能推荐助手Demo（AI领域）" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/HyCjwOFsoirEEnkJnddcEwo0noh?from=from_copylink"/>
-    <hyperlink ref="C23" r:id="rId12" display="一周构建智能信贷报告生成系统Demo" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/WzlLwUPYFiaUiYkTl4LcIaBCnyf?from=from_copylink"/>
-    <hyperlink ref="C24" r:id="rId13" display="一周构建单条全国产业链图谱" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/HfZEwCQKAis15tk01CzcjabYnOf?from=from_copylink"/>
+    <hyperlink ref="C4" r:id="rId1" display="智能调研报告生成" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/DbbUwFE8FiYjupki6uzcRqT0nEe?from=from_copylink"/>
+    <hyperlink ref="C6" r:id="rId2" display="业务看板搭建" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/CtjuwGhsIiE977kD7TLc4u0KnRe?from=from_copylink"/>
+    <hyperlink ref="C7" r:id="rId3" display="文档审核与风控" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/PQ6MwPExLi3v2Vkn3DAckYxGn8b?from=from_copylink"/>
+    <hyperlink ref="C9" r:id="rId4" display="企业演示视频" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/Dkl8wQ6fBiE49Gk4XE2cTRc2nhD?from=from_copylink"/>
+    <hyperlink ref="C11" r:id="rId5" display="儿童教育趣味应用" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/Csk3wFuMwiZk00kt8WJco88Wn5g?from=from_copylink"/>
+    <hyperlink ref="C13" r:id="rId6" display="长时间序列预测系统" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/G6S3wY1eriHk3UkfCDlc6PEznpd?from=from_copylink"/>
+    <hyperlink ref="C15" r:id="rId7" display="智能文档翻译系统" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/QHljw6HhbiceMPkBC49cmvzNnXf?from=from_copylink"/>
+    <hyperlink ref="C17" r:id="rId8" display="智能合同法审系统" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/NfpfwmK16iXEDtkznIscn549nEb?from=from_copylink"/>
+    <hyperlink ref="C19" r:id="rId9" display="通用目标检测系统" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/OfMfwwUxMic5Qkkul8GcaA5En4d?from=from_copylink"/>
+    <hyperlink ref="C20" r:id="rId10" display="SQL语言智能生成" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/GGMKw7bP7iXmNpk88OxcsqCznmg?from=from_copylink"/>
+    <hyperlink ref="C21" r:id="rId11" display="功能推荐助手" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/HyCjwOFsoirEEnkJnddcEwo0noh?from=from_copylink"/>
+    <hyperlink ref="C23" r:id="rId12" display="智能信贷报告生成系统" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/WzlLwUPYFiaUiYkTl4LcIaBCnyf?from=from_copylink"/>
+    <hyperlink ref="C24" r:id="rId13" display="单条产业链图谱" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/HfZEwCQKAis15tk01CzcjabYnOf?from=from_copylink"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
fix: resolve JSX parsing errors and fix navigation issues
- Fix JSX parsing errors by replacing template literals with string concatenation in className attributes
- Fix homepage "Browse Best Practices" button to include locale prefix (/arena → /${locale}/arena)
- Fix "View Full Implementation Details" button to scroll to top instead of using hash anchor
- Fix version status display to show full date (YYYY-MM-DD) instead of just year
- Update content files for i18n consistency

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Content/Arena/List of Arenas.xlsx
+++ b/Content/Arena/List of Arenas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255"/>
+    <workbookView windowWidth="19515" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
   <si>
     <t>擂台编号</t>
   </si>
@@ -64,6 +64,9 @@
     <t>成本</t>
   </si>
   <si>
+    <t>攻擂中</t>
+  </si>
+  <si>
     <t>智能调研报告生成</t>
   </si>
   <si>
@@ -231,6 +234,20 @@
     <t>较优</t>
   </si>
   <si>
+    <r>
+      <t>私部署版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Claude Code + Kimi K2.5 + Metaso</t>
+    </r>
+  </si>
+  <si>
     <t>业务看板搭建</t>
   </si>
   <si>
@@ -378,6 +395,20 @@
     <t>较低</t>
   </si>
   <si>
+    <r>
+      <t>云端版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Lovable + Kimi K2.5 + Claude Code</t>
+    </r>
+  </si>
+  <si>
     <t>文档审核与风控</t>
   </si>
   <si>
@@ -551,6 +582,20 @@
     </r>
   </si>
   <si>
+    <r>
+      <t>私部署版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>LangChain + Kimi K2.5 + Pydantic + unstructured + Faiss</t>
+    </r>
+  </si>
+  <si>
     <t>企业演示视频</t>
   </si>
   <si>
@@ -653,6 +698,20 @@
     <t>中等</t>
   </si>
   <si>
+    <r>
+      <t>私部署版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Claude Code + Kimi K2.5 + FFmpeg + FunASR + PaddleSpeech</t>
+    </r>
+  </si>
+  <si>
     <t>儿童教育趣味应用</t>
   </si>
   <si>
@@ -728,6 +787,20 @@
     <t>服务</t>
   </si>
   <si>
+    <r>
+      <t>私部署版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">BISHENG + Kimi K2.5 </t>
+    </r>
+  </si>
+  <si>
     <t>长时间序列预测系统</t>
   </si>
   <si>
@@ -803,6 +876,9 @@
     </r>
   </si>
   <si>
+    <t>寻找攻擂者</t>
+  </si>
+  <si>
     <t>智能文档翻译系统</t>
   </si>
   <si>
@@ -1307,6 +1383,20 @@
     </r>
   </si>
   <si>
+    <r>
+      <t>私部署版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Coze + Kimi K2.5 </t>
+    </r>
+  </si>
+  <si>
     <t>智能信贷报告生成系统</t>
   </si>
   <si>
@@ -1347,6 +1437,20 @@
         <charset val="134"/>
       </rPr>
       <t>Demo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>私部署版：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">LangChain + Kimi K2.5 </t>
     </r>
   </si>
   <si>
@@ -2456,19 +2560,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:L25"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="4" max="4" width="23.2583333333333" customWidth="1"/>
+    <col min="13" max="13" width="23.2583333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="15" customHeight="1"/>
-    <row r="3" ht="15" spans="2:12">
+    <row r="3" ht="15" spans="2:13">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2502,43 +2607,49 @@
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:13">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="2:12">
+    <row r="5" ht="15" customHeight="1" spans="2:13">
       <c r="B5" s="3"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
@@ -2550,78 +2661,85 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
     </row>
-    <row r="6" ht="114.75" spans="2:12">
+    <row r="6" ht="114.75" spans="2:13">
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>19</v>
+      <c r="M6" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="7" ht="143.25" customHeight="1" spans="2:12">
+    <row r="7" ht="143.25" customHeight="1" spans="2:13">
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="2:12">
+    <row r="8" spans="2:13">
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
       <c r="D8" s="6"/>
@@ -2633,43 +2751,47 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
-    <row r="9" ht="157.5" customHeight="1" spans="2:12">
+    <row r="9" ht="157.5" customHeight="1" spans="2:13">
       <c r="B9" s="3">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="10" ht="14.25" spans="2:12">
+    <row r="10" spans="2:13">
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -2681,43 +2803,47 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
     </row>
-    <row r="11" ht="72" customHeight="1" spans="2:12">
+    <row r="11" ht="72" customHeight="1" spans="2:13">
       <c r="B11" s="3">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="K11" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="12" ht="14.25" spans="2:12">
+    <row r="12" spans="2:13">
       <c r="B12" s="3"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
@@ -2729,43 +2855,47 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
-    <row r="13" ht="129" customHeight="1" spans="2:12">
+    <row r="13" ht="129" customHeight="1" spans="2:13">
       <c r="B13" s="3">
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="14" ht="14.25" spans="2:12">
+    <row r="14" spans="2:13">
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
@@ -2777,43 +2907,47 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
     </row>
-    <row r="15" ht="114.75" customHeight="1" spans="2:12">
+    <row r="15" ht="114.75" customHeight="1" spans="2:13">
       <c r="B15" s="3">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="16" ht="14.25" spans="2:12">
+    <row r="16" ht="14.25" spans="2:13">
       <c r="B16" s="3"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
@@ -2825,43 +2959,47 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:13">
       <c r="B17" s="3">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="18" ht="14.25" spans="2:12">
+    <row r="18" spans="2:13">
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="6"/>
@@ -2873,113 +3011,123 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
-    <row r="19" ht="201" customHeight="1" spans="2:12">
+    <row r="19" ht="201" customHeight="1" spans="2:13">
       <c r="B19">
         <v>9</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="20" ht="72" spans="2:12">
+    <row r="20" ht="72" spans="2:13">
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:13">
       <c r="B21" s="3">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="22" ht="14.25" spans="2:12">
+    <row r="22" spans="2:13">
       <c r="B22" s="3"/>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
@@ -2991,83 +3139,90 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
     </row>
-    <row r="23" ht="157.5" spans="2:12">
+    <row r="23" ht="157.5" spans="2:13">
       <c r="B23">
         <v>12</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="24" ht="86.25" spans="2:12">
+    <row r="24" ht="86.25" spans="2:13">
       <c r="B24">
         <v>13</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="25" ht="29.25" spans="2:12">
+    <row r="25" ht="29.25" spans="2:13">
       <c r="B25">
         <v>14</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3078,9 +3233,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
+      <c r="M25" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="88">
+  <mergeCells count="96">
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
@@ -3169,6 +3325,14 @@
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="智能调研报告生成" tooltip="https://gvxnc4ekbvn.feishu.cn/wiki/DbbUwFE8FiYjupki6uzcRqT0nEe?from=from_copylink"/>

</xml_diff>